<commit_message>
Update .xlsx file and DataXLSXtraction.cpp
Add a void cell to test with void cell.
Starting to check what cell is currently traiting
</commit_message>
<xml_diff>
--- a/thinkingAbout/test.xlsx
+++ b/thinkingAbout/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewee\JetBrainsProjects\CLion\Kuesto\thinkingAbout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBCF321-67B6-4678-A157-E9EFC352DD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49D4A7C3-9913-45C3-B2BD-95554C35F9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{827586CA-356A-4DF1-9C87-459289FC3A72}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,12 +37,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>sheet 1</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>rien en cell A4</t>
+  </si>
   <si>
     <t>I'm</t>
-  </si>
-  <si>
-    <t>sheet 1</t>
   </si>
   <si>
     <t>sheet 2</t>
@@ -48,15 +56,12 @@
   <si>
     <t>[2]</t>
   </si>
-  <si>
-    <t>Column</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,7 +165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -456,27 +461,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C267AA-F747-4546-B487-C239BAF1B767}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="120" customWidth="1"/>
     <col min="2" max="2" width="118.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,7 +489,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="348.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" ht="348.75" customHeight="1"/>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -499,26 +509,26 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>